<commit_message>
edit the sl fmri experiment stimuli
</commit_message>
<xml_diff>
--- a/experiments/sl-fmri-expt/dec2018_fmri/visual/visual_run1.xlsx
+++ b/experiments/sl-fmri-expt/dec2018_fmri/visual/visual_run1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qlab\Documents\new_fmri\visual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brainstim\Documents\modified_fmri\modified_fmri\modified_visual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="ssl_run1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="34">
   <si>
     <t>trialnum</t>
   </si>
@@ -927,9 +927,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F481"/>
+  <dimension ref="A1:F349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7913,2646 +7915,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>20</v>
-      </c>
-      <c r="B350">
-        <v>0</v>
-      </c>
-      <c r="C350" t="s">
-        <v>6</v>
-      </c>
-      <c r="D350">
-        <v>0</v>
-      </c>
-      <c r="E350">
-        <v>0</v>
-      </c>
-      <c r="F350">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>20</v>
-      </c>
-      <c r="B351">
-        <v>0</v>
-      </c>
-      <c r="C351" t="s">
-        <v>6</v>
-      </c>
-      <c r="D351">
-        <v>0</v>
-      </c>
-      <c r="E351">
-        <v>0</v>
-      </c>
-      <c r="F351">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>20</v>
-      </c>
-      <c r="B352">
-        <v>0</v>
-      </c>
-      <c r="C352" t="s">
-        <v>6</v>
-      </c>
-      <c r="D352">
-        <v>0</v>
-      </c>
-      <c r="E352">
-        <v>0</v>
-      </c>
-      <c r="F352">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>20</v>
-      </c>
-      <c r="B353">
-        <v>0</v>
-      </c>
-      <c r="C353" t="s">
-        <v>6</v>
-      </c>
-      <c r="D353">
-        <v>0</v>
-      </c>
-      <c r="E353">
-        <v>0</v>
-      </c>
-      <c r="F353">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
-        <v>20</v>
-      </c>
-      <c r="B354">
-        <v>0</v>
-      </c>
-      <c r="C354" t="s">
-        <v>6</v>
-      </c>
-      <c r="D354">
-        <v>0</v>
-      </c>
-      <c r="E354">
-        <v>0</v>
-      </c>
-      <c r="F354">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
-        <v>20</v>
-      </c>
-      <c r="B355">
-        <v>0</v>
-      </c>
-      <c r="C355" t="s">
-        <v>6</v>
-      </c>
-      <c r="D355">
-        <v>0</v>
-      </c>
-      <c r="E355">
-        <v>0</v>
-      </c>
-      <c r="F355">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>20</v>
-      </c>
-      <c r="B356">
-        <v>0</v>
-      </c>
-      <c r="C356" t="s">
-        <v>6</v>
-      </c>
-      <c r="D356">
-        <v>0</v>
-      </c>
-      <c r="E356">
-        <v>0</v>
-      </c>
-      <c r="F356">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>20</v>
-      </c>
-      <c r="B357">
-        <v>0</v>
-      </c>
-      <c r="C357" t="s">
-        <v>6</v>
-      </c>
-      <c r="D357">
-        <v>0</v>
-      </c>
-      <c r="E357">
-        <v>0</v>
-      </c>
-      <c r="F357">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
-        <v>20</v>
-      </c>
-      <c r="B358">
-        <v>0</v>
-      </c>
-      <c r="C358" t="s">
-        <v>6</v>
-      </c>
-      <c r="D358">
-        <v>0</v>
-      </c>
-      <c r="E358">
-        <v>0</v>
-      </c>
-      <c r="F358">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
-        <v>20</v>
-      </c>
-      <c r="B359">
-        <v>0</v>
-      </c>
-      <c r="C359" t="s">
-        <v>6</v>
-      </c>
-      <c r="D359">
-        <v>0</v>
-      </c>
-      <c r="E359">
-        <v>0</v>
-      </c>
-      <c r="F359">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
-        <v>20</v>
-      </c>
-      <c r="B360">
-        <v>0</v>
-      </c>
-      <c r="C360" t="s">
-        <v>6</v>
-      </c>
-      <c r="D360">
-        <v>0</v>
-      </c>
-      <c r="E360">
-        <v>0</v>
-      </c>
-      <c r="F360">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>20</v>
-      </c>
-      <c r="B361">
-        <v>0</v>
-      </c>
-      <c r="C361" t="s">
-        <v>6</v>
-      </c>
-      <c r="D361">
-        <v>0</v>
-      </c>
-      <c r="E361">
-        <v>0</v>
-      </c>
-      <c r="F361">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>31</v>
-      </c>
-      <c r="B362">
-        <v>145</v>
-      </c>
-      <c r="C362" t="s">
-        <v>7</v>
-      </c>
-      <c r="D362">
-        <v>0</v>
-      </c>
-      <c r="E362">
-        <v>1</v>
-      </c>
-      <c r="F362">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>22</v>
-      </c>
-      <c r="B363">
-        <v>146</v>
-      </c>
-      <c r="C363" t="s">
-        <v>7</v>
-      </c>
-      <c r="D363">
-        <v>0</v>
-      </c>
-      <c r="E363">
-        <v>2</v>
-      </c>
-      <c r="F363">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>22</v>
-      </c>
-      <c r="B364">
-        <v>147</v>
-      </c>
-      <c r="C364" t="s">
-        <v>7</v>
-      </c>
-      <c r="D364">
-        <v>0</v>
-      </c>
-      <c r="E364">
-        <v>3</v>
-      </c>
-      <c r="F364">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
-        <v>25</v>
-      </c>
-      <c r="B365">
-        <v>148</v>
-      </c>
-      <c r="C365" t="s">
-        <v>7</v>
-      </c>
-      <c r="D365">
-        <v>0</v>
-      </c>
-      <c r="E365">
-        <v>1</v>
-      </c>
-      <c r="F365">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
-        <v>26</v>
-      </c>
-      <c r="B366">
-        <v>149</v>
-      </c>
-      <c r="C366" t="s">
-        <v>7</v>
-      </c>
-      <c r="D366">
-        <v>0</v>
-      </c>
-      <c r="E366">
-        <v>2</v>
-      </c>
-      <c r="F366">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
-        <v>27</v>
-      </c>
-      <c r="B367">
-        <v>150</v>
-      </c>
-      <c r="C367" t="s">
-        <v>7</v>
-      </c>
-      <c r="D367">
-        <v>0</v>
-      </c>
-      <c r="E367">
-        <v>3</v>
-      </c>
-      <c r="F367">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
-        <v>32</v>
-      </c>
-      <c r="B368">
-        <v>151</v>
-      </c>
-      <c r="C368" t="s">
-        <v>7</v>
-      </c>
-      <c r="D368">
-        <v>0</v>
-      </c>
-      <c r="E368">
-        <v>1</v>
-      </c>
-      <c r="F368">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
-        <v>23</v>
-      </c>
-      <c r="B369">
-        <v>152</v>
-      </c>
-      <c r="C369" t="s">
-        <v>7</v>
-      </c>
-      <c r="D369">
-        <v>0</v>
-      </c>
-      <c r="E369">
-        <v>2</v>
-      </c>
-      <c r="F369">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
-        <v>23</v>
-      </c>
-      <c r="B370">
-        <v>153</v>
-      </c>
-      <c r="C370" t="s">
-        <v>7</v>
-      </c>
-      <c r="D370">
-        <v>0</v>
-      </c>
-      <c r="E370">
-        <v>3</v>
-      </c>
-      <c r="F370">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
-        <v>23</v>
-      </c>
-      <c r="B371">
-        <v>154</v>
-      </c>
-      <c r="C371" t="s">
-        <v>7</v>
-      </c>
-      <c r="D371">
-        <v>0</v>
-      </c>
-      <c r="E371">
-        <v>1</v>
-      </c>
-      <c r="F371">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
-        <v>28</v>
-      </c>
-      <c r="B372">
-        <v>155</v>
-      </c>
-      <c r="C372" t="s">
-        <v>7</v>
-      </c>
-      <c r="D372">
-        <v>0</v>
-      </c>
-      <c r="E372">
-        <v>2</v>
-      </c>
-      <c r="F372">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A373" t="s">
-        <v>32</v>
-      </c>
-      <c r="B373">
-        <v>156</v>
-      </c>
-      <c r="C373" t="s">
-        <v>7</v>
-      </c>
-      <c r="D373">
-        <v>0</v>
-      </c>
-      <c r="E373">
-        <v>3</v>
-      </c>
-      <c r="F373">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
-        <v>26</v>
-      </c>
-      <c r="B374">
-        <v>157</v>
-      </c>
-      <c r="C374" t="s">
-        <v>7</v>
-      </c>
-      <c r="D374">
-        <v>0</v>
-      </c>
-      <c r="E374">
-        <v>1</v>
-      </c>
-      <c r="F374">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
-        <v>22</v>
-      </c>
-      <c r="B375">
-        <v>158</v>
-      </c>
-      <c r="C375" t="s">
-        <v>7</v>
-      </c>
-      <c r="D375">
-        <v>0</v>
-      </c>
-      <c r="E375">
-        <v>2</v>
-      </c>
-      <c r="F375">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
-        <v>29</v>
-      </c>
-      <c r="B376">
-        <v>159</v>
-      </c>
-      <c r="C376" t="s">
-        <v>7</v>
-      </c>
-      <c r="D376">
-        <v>0</v>
-      </c>
-      <c r="E376">
-        <v>3</v>
-      </c>
-      <c r="F376">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
-        <v>30</v>
-      </c>
-      <c r="B377">
-        <v>160</v>
-      </c>
-      <c r="C377" t="s">
-        <v>7</v>
-      </c>
-      <c r="D377">
-        <v>0</v>
-      </c>
-      <c r="E377">
-        <v>1</v>
-      </c>
-      <c r="F377">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
-        <v>31</v>
-      </c>
-      <c r="B378">
-        <v>161</v>
-      </c>
-      <c r="C378" t="s">
-        <v>7</v>
-      </c>
-      <c r="D378">
-        <v>0</v>
-      </c>
-      <c r="E378">
-        <v>2</v>
-      </c>
-      <c r="F378">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
-        <v>28</v>
-      </c>
-      <c r="B379">
-        <v>162</v>
-      </c>
-      <c r="C379" t="s">
-        <v>7</v>
-      </c>
-      <c r="D379">
-        <v>0</v>
-      </c>
-      <c r="E379">
-        <v>3</v>
-      </c>
-      <c r="F379">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
-        <v>21</v>
-      </c>
-      <c r="B380">
-        <v>163</v>
-      </c>
-      <c r="C380" t="s">
-        <v>7</v>
-      </c>
-      <c r="D380">
-        <v>0</v>
-      </c>
-      <c r="E380">
-        <v>1</v>
-      </c>
-      <c r="F380">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
-        <v>21</v>
-      </c>
-      <c r="B381">
-        <v>164</v>
-      </c>
-      <c r="C381" t="s">
-        <v>7</v>
-      </c>
-      <c r="D381">
-        <v>0</v>
-      </c>
-      <c r="E381">
-        <v>2</v>
-      </c>
-      <c r="F381">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
-        <v>25</v>
-      </c>
-      <c r="B382">
-        <v>165</v>
-      </c>
-      <c r="C382" t="s">
-        <v>7</v>
-      </c>
-      <c r="D382">
-        <v>0</v>
-      </c>
-      <c r="E382">
-        <v>3</v>
-      </c>
-      <c r="F382">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
-        <v>29</v>
-      </c>
-      <c r="B383">
-        <v>166</v>
-      </c>
-      <c r="C383" t="s">
-        <v>7</v>
-      </c>
-      <c r="D383">
-        <v>0</v>
-      </c>
-      <c r="E383">
-        <v>1</v>
-      </c>
-      <c r="F383">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
-        <v>24</v>
-      </c>
-      <c r="B384">
-        <v>167</v>
-      </c>
-      <c r="C384" t="s">
-        <v>7</v>
-      </c>
-      <c r="D384">
-        <v>0</v>
-      </c>
-      <c r="E384">
-        <v>2</v>
-      </c>
-      <c r="F384">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
-        <v>29</v>
-      </c>
-      <c r="B385">
-        <v>168</v>
-      </c>
-      <c r="C385" t="s">
-        <v>7</v>
-      </c>
-      <c r="D385">
-        <v>0</v>
-      </c>
-      <c r="E385">
-        <v>3</v>
-      </c>
-      <c r="F385">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
-        <v>8</v>
-      </c>
-      <c r="B386">
-        <v>145</v>
-      </c>
-      <c r="C386" t="s">
-        <v>5</v>
-      </c>
-      <c r="D386">
-        <v>1</v>
-      </c>
-      <c r="E386">
-        <v>1</v>
-      </c>
-      <c r="F386">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
-        <v>9</v>
-      </c>
-      <c r="B387">
-        <v>146</v>
-      </c>
-      <c r="C387" t="s">
-        <v>5</v>
-      </c>
-      <c r="D387">
-        <v>1</v>
-      </c>
-      <c r="E387">
-        <v>2</v>
-      </c>
-      <c r="F387">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>10</v>
-      </c>
-      <c r="B388">
-        <v>147</v>
-      </c>
-      <c r="C388" t="s">
-        <v>5</v>
-      </c>
-      <c r="D388">
-        <v>1</v>
-      </c>
-      <c r="E388">
-        <v>3</v>
-      </c>
-      <c r="F388">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
-        <v>17</v>
-      </c>
-      <c r="B389">
-        <v>148</v>
-      </c>
-      <c r="C389" t="s">
-        <v>5</v>
-      </c>
-      <c r="D389">
-        <v>3</v>
-      </c>
-      <c r="E389">
-        <v>1</v>
-      </c>
-      <c r="F389">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
-        <v>18</v>
-      </c>
-      <c r="B390">
-        <v>149</v>
-      </c>
-      <c r="C390" t="s">
-        <v>5</v>
-      </c>
-      <c r="D390">
-        <v>3</v>
-      </c>
-      <c r="E390">
-        <v>2</v>
-      </c>
-      <c r="F390">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>19</v>
-      </c>
-      <c r="B391">
-        <v>150</v>
-      </c>
-      <c r="C391" t="s">
-        <v>5</v>
-      </c>
-      <c r="D391">
-        <v>3</v>
-      </c>
-      <c r="E391">
-        <v>3</v>
-      </c>
-      <c r="F391">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
-        <v>8</v>
-      </c>
-      <c r="B392">
-        <v>151</v>
-      </c>
-      <c r="C392" t="s">
-        <v>5</v>
-      </c>
-      <c r="D392">
-        <v>1</v>
-      </c>
-      <c r="E392">
-        <v>1</v>
-      </c>
-      <c r="F392">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
-        <v>9</v>
-      </c>
-      <c r="B393">
-        <v>152</v>
-      </c>
-      <c r="C393" t="s">
-        <v>5</v>
-      </c>
-      <c r="D393">
-        <v>1</v>
-      </c>
-      <c r="E393">
-        <v>2</v>
-      </c>
-      <c r="F393">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
-        <v>10</v>
-      </c>
-      <c r="B394">
-        <v>153</v>
-      </c>
-      <c r="C394" t="s">
-        <v>5</v>
-      </c>
-      <c r="D394">
-        <v>1</v>
-      </c>
-      <c r="E394">
-        <v>3</v>
-      </c>
-      <c r="F394">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
-        <v>14</v>
-      </c>
-      <c r="B395">
-        <v>154</v>
-      </c>
-      <c r="C395" t="s">
-        <v>5</v>
-      </c>
-      <c r="D395">
-        <v>4</v>
-      </c>
-      <c r="E395">
-        <v>1</v>
-      </c>
-      <c r="F395">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
-        <v>15</v>
-      </c>
-      <c r="B396">
-        <v>155</v>
-      </c>
-      <c r="C396" t="s">
-        <v>5</v>
-      </c>
-      <c r="D396">
-        <v>4</v>
-      </c>
-      <c r="E396">
-        <v>2</v>
-      </c>
-      <c r="F396">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A397" t="s">
-        <v>16</v>
-      </c>
-      <c r="B397">
-        <v>156</v>
-      </c>
-      <c r="C397" t="s">
-        <v>5</v>
-      </c>
-      <c r="D397">
-        <v>4</v>
-      </c>
-      <c r="E397">
-        <v>3</v>
-      </c>
-      <c r="F397">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
-        <v>11</v>
-      </c>
-      <c r="B398">
-        <v>157</v>
-      </c>
-      <c r="C398" t="s">
-        <v>5</v>
-      </c>
-      <c r="D398">
-        <v>2</v>
-      </c>
-      <c r="E398">
-        <v>1</v>
-      </c>
-      <c r="F398">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>12</v>
-      </c>
-      <c r="B399">
-        <v>158</v>
-      </c>
-      <c r="C399" t="s">
-        <v>5</v>
-      </c>
-      <c r="D399">
-        <v>2</v>
-      </c>
-      <c r="E399">
-        <v>2</v>
-      </c>
-      <c r="F399">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
-        <v>13</v>
-      </c>
-      <c r="B400">
-        <v>159</v>
-      </c>
-      <c r="C400" t="s">
-        <v>5</v>
-      </c>
-      <c r="D400">
-        <v>2</v>
-      </c>
-      <c r="E400">
-        <v>3</v>
-      </c>
-      <c r="F400">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A401" t="s">
-        <v>8</v>
-      </c>
-      <c r="B401">
-        <v>160</v>
-      </c>
-      <c r="C401" t="s">
-        <v>5</v>
-      </c>
-      <c r="D401">
-        <v>1</v>
-      </c>
-      <c r="E401">
-        <v>1</v>
-      </c>
-      <c r="F401">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A402" t="s">
-        <v>9</v>
-      </c>
-      <c r="B402">
-        <v>161</v>
-      </c>
-      <c r="C402" t="s">
-        <v>5</v>
-      </c>
-      <c r="D402">
-        <v>1</v>
-      </c>
-      <c r="E402">
-        <v>2</v>
-      </c>
-      <c r="F402">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
-        <v>10</v>
-      </c>
-      <c r="B403">
-        <v>162</v>
-      </c>
-      <c r="C403" t="s">
-        <v>5</v>
-      </c>
-      <c r="D403">
-        <v>1</v>
-      </c>
-      <c r="E403">
-        <v>3</v>
-      </c>
-      <c r="F403">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A404" t="s">
-        <v>14</v>
-      </c>
-      <c r="B404">
-        <v>163</v>
-      </c>
-      <c r="C404" t="s">
-        <v>5</v>
-      </c>
-      <c r="D404">
-        <v>4</v>
-      </c>
-      <c r="E404">
-        <v>1</v>
-      </c>
-      <c r="F404">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A405" t="s">
-        <v>15</v>
-      </c>
-      <c r="B405">
-        <v>164</v>
-      </c>
-      <c r="C405" t="s">
-        <v>5</v>
-      </c>
-      <c r="D405">
-        <v>4</v>
-      </c>
-      <c r="E405">
-        <v>2</v>
-      </c>
-      <c r="F405">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A406" t="s">
-        <v>16</v>
-      </c>
-      <c r="B406">
-        <v>165</v>
-      </c>
-      <c r="C406" t="s">
-        <v>5</v>
-      </c>
-      <c r="D406">
-        <v>4</v>
-      </c>
-      <c r="E406">
-        <v>3</v>
-      </c>
-      <c r="F406">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A407" t="s">
-        <v>11</v>
-      </c>
-      <c r="B407">
-        <v>166</v>
-      </c>
-      <c r="C407" t="s">
-        <v>5</v>
-      </c>
-      <c r="D407">
-        <v>2</v>
-      </c>
-      <c r="E407">
-        <v>1</v>
-      </c>
-      <c r="F407">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A408" t="s">
-        <v>12</v>
-      </c>
-      <c r="B408">
-        <v>167</v>
-      </c>
-      <c r="C408" t="s">
-        <v>5</v>
-      </c>
-      <c r="D408">
-        <v>2</v>
-      </c>
-      <c r="E408">
-        <v>2</v>
-      </c>
-      <c r="F408">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>13</v>
-      </c>
-      <c r="B409">
-        <v>168</v>
-      </c>
-      <c r="C409" t="s">
-        <v>5</v>
-      </c>
-      <c r="D409">
-        <v>2</v>
-      </c>
-      <c r="E409">
-        <v>3</v>
-      </c>
-      <c r="F409">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A410" t="s">
-        <v>20</v>
-      </c>
-      <c r="B410">
-        <v>0</v>
-      </c>
-      <c r="C410" t="s">
-        <v>6</v>
-      </c>
-      <c r="D410">
-        <v>0</v>
-      </c>
-      <c r="E410">
-        <v>0</v>
-      </c>
-      <c r="F410">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A411" t="s">
-        <v>20</v>
-      </c>
-      <c r="B411">
-        <v>0</v>
-      </c>
-      <c r="C411" t="s">
-        <v>6</v>
-      </c>
-      <c r="D411">
-        <v>0</v>
-      </c>
-      <c r="E411">
-        <v>0</v>
-      </c>
-      <c r="F411">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A412" t="s">
-        <v>20</v>
-      </c>
-      <c r="B412">
-        <v>0</v>
-      </c>
-      <c r="C412" t="s">
-        <v>6</v>
-      </c>
-      <c r="D412">
-        <v>0</v>
-      </c>
-      <c r="E412">
-        <v>0</v>
-      </c>
-      <c r="F412">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A413" t="s">
-        <v>20</v>
-      </c>
-      <c r="B413">
-        <v>0</v>
-      </c>
-      <c r="C413" t="s">
-        <v>6</v>
-      </c>
-      <c r="D413">
-        <v>0</v>
-      </c>
-      <c r="E413">
-        <v>0</v>
-      </c>
-      <c r="F413">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A414" t="s">
-        <v>20</v>
-      </c>
-      <c r="B414">
-        <v>0</v>
-      </c>
-      <c r="C414" t="s">
-        <v>6</v>
-      </c>
-      <c r="D414">
-        <v>0</v>
-      </c>
-      <c r="E414">
-        <v>0</v>
-      </c>
-      <c r="F414">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A415" t="s">
-        <v>20</v>
-      </c>
-      <c r="B415">
-        <v>0</v>
-      </c>
-      <c r="C415" t="s">
-        <v>6</v>
-      </c>
-      <c r="D415">
-        <v>0</v>
-      </c>
-      <c r="E415">
-        <v>0</v>
-      </c>
-      <c r="F415">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A416" t="s">
-        <v>20</v>
-      </c>
-      <c r="B416">
-        <v>0</v>
-      </c>
-      <c r="C416" t="s">
-        <v>6</v>
-      </c>
-      <c r="D416">
-        <v>0</v>
-      </c>
-      <c r="E416">
-        <v>0</v>
-      </c>
-      <c r="F416">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A417" t="s">
-        <v>20</v>
-      </c>
-      <c r="B417">
-        <v>0</v>
-      </c>
-      <c r="C417" t="s">
-        <v>6</v>
-      </c>
-      <c r="D417">
-        <v>0</v>
-      </c>
-      <c r="E417">
-        <v>0</v>
-      </c>
-      <c r="F417">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
-        <v>20</v>
-      </c>
-      <c r="B418">
-        <v>0</v>
-      </c>
-      <c r="C418" t="s">
-        <v>6</v>
-      </c>
-      <c r="D418">
-        <v>0</v>
-      </c>
-      <c r="E418">
-        <v>0</v>
-      </c>
-      <c r="F418">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A419" t="s">
-        <v>20</v>
-      </c>
-      <c r="B419">
-        <v>0</v>
-      </c>
-      <c r="C419" t="s">
-        <v>6</v>
-      </c>
-      <c r="D419">
-        <v>0</v>
-      </c>
-      <c r="E419">
-        <v>0</v>
-      </c>
-      <c r="F419">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A420" t="s">
-        <v>20</v>
-      </c>
-      <c r="B420">
-        <v>0</v>
-      </c>
-      <c r="C420" t="s">
-        <v>6</v>
-      </c>
-      <c r="D420">
-        <v>0</v>
-      </c>
-      <c r="E420">
-        <v>0</v>
-      </c>
-      <c r="F420">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A421" t="s">
-        <v>20</v>
-      </c>
-      <c r="B421">
-        <v>0</v>
-      </c>
-      <c r="C421" t="s">
-        <v>6</v>
-      </c>
-      <c r="D421">
-        <v>0</v>
-      </c>
-      <c r="E421">
-        <v>0</v>
-      </c>
-      <c r="F421">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A422" t="s">
-        <v>17</v>
-      </c>
-      <c r="B422">
-        <v>169</v>
-      </c>
-      <c r="C422" t="s">
-        <v>5</v>
-      </c>
-      <c r="D422">
-        <v>3</v>
-      </c>
-      <c r="E422">
-        <v>1</v>
-      </c>
-      <c r="F422">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A423" t="s">
-        <v>18</v>
-      </c>
-      <c r="B423">
-        <v>170</v>
-      </c>
-      <c r="C423" t="s">
-        <v>5</v>
-      </c>
-      <c r="D423">
-        <v>3</v>
-      </c>
-      <c r="E423">
-        <v>2</v>
-      </c>
-      <c r="F423">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>19</v>
-      </c>
-      <c r="B424">
-        <v>171</v>
-      </c>
-      <c r="C424" t="s">
-        <v>5</v>
-      </c>
-      <c r="D424">
-        <v>3</v>
-      </c>
-      <c r="E424">
-        <v>3</v>
-      </c>
-      <c r="F424">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
-        <v>11</v>
-      </c>
-      <c r="B425">
-        <v>172</v>
-      </c>
-      <c r="C425" t="s">
-        <v>5</v>
-      </c>
-      <c r="D425">
-        <v>2</v>
-      </c>
-      <c r="E425">
-        <v>1</v>
-      </c>
-      <c r="F425">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A426" t="s">
-        <v>12</v>
-      </c>
-      <c r="B426">
-        <v>173</v>
-      </c>
-      <c r="C426" t="s">
-        <v>5</v>
-      </c>
-      <c r="D426">
-        <v>2</v>
-      </c>
-      <c r="E426">
-        <v>2</v>
-      </c>
-      <c r="F426">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A427" t="s">
-        <v>13</v>
-      </c>
-      <c r="B427">
-        <v>174</v>
-      </c>
-      <c r="C427" t="s">
-        <v>5</v>
-      </c>
-      <c r="D427">
-        <v>2</v>
-      </c>
-      <c r="E427">
-        <v>3</v>
-      </c>
-      <c r="F427">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
-        <v>8</v>
-      </c>
-      <c r="B428">
-        <v>175</v>
-      </c>
-      <c r="C428" t="s">
-        <v>5</v>
-      </c>
-      <c r="D428">
-        <v>1</v>
-      </c>
-      <c r="E428">
-        <v>1</v>
-      </c>
-      <c r="F428">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
-        <v>9</v>
-      </c>
-      <c r="B429">
-        <v>176</v>
-      </c>
-      <c r="C429" t="s">
-        <v>5</v>
-      </c>
-      <c r="D429">
-        <v>1</v>
-      </c>
-      <c r="E429">
-        <v>2</v>
-      </c>
-      <c r="F429">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A430" t="s">
-        <v>10</v>
-      </c>
-      <c r="B430">
-        <v>177</v>
-      </c>
-      <c r="C430" t="s">
-        <v>5</v>
-      </c>
-      <c r="D430">
-        <v>1</v>
-      </c>
-      <c r="E430">
-        <v>3</v>
-      </c>
-      <c r="F430">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A431" t="s">
-        <v>17</v>
-      </c>
-      <c r="B431">
-        <v>178</v>
-      </c>
-      <c r="C431" t="s">
-        <v>5</v>
-      </c>
-      <c r="D431">
-        <v>3</v>
-      </c>
-      <c r="E431">
-        <v>1</v>
-      </c>
-      <c r="F431">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A432" t="s">
-        <v>18</v>
-      </c>
-      <c r="B432">
-        <v>179</v>
-      </c>
-      <c r="C432" t="s">
-        <v>5</v>
-      </c>
-      <c r="D432">
-        <v>3</v>
-      </c>
-      <c r="E432">
-        <v>2</v>
-      </c>
-      <c r="F432">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A433" t="s">
-        <v>19</v>
-      </c>
-      <c r="B433">
-        <v>180</v>
-      </c>
-      <c r="C433" t="s">
-        <v>5</v>
-      </c>
-      <c r="D433">
-        <v>3</v>
-      </c>
-      <c r="E433">
-        <v>3</v>
-      </c>
-      <c r="F433">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A434" t="s">
-        <v>14</v>
-      </c>
-      <c r="B434">
-        <v>181</v>
-      </c>
-      <c r="C434" t="s">
-        <v>5</v>
-      </c>
-      <c r="D434">
-        <v>4</v>
-      </c>
-      <c r="E434">
-        <v>1</v>
-      </c>
-      <c r="F434">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
-        <v>15</v>
-      </c>
-      <c r="B435">
-        <v>182</v>
-      </c>
-      <c r="C435" t="s">
-        <v>5</v>
-      </c>
-      <c r="D435">
-        <v>4</v>
-      </c>
-      <c r="E435">
-        <v>2</v>
-      </c>
-      <c r="F435">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A436" t="s">
-        <v>16</v>
-      </c>
-      <c r="B436">
-        <v>183</v>
-      </c>
-      <c r="C436" t="s">
-        <v>5</v>
-      </c>
-      <c r="D436">
-        <v>4</v>
-      </c>
-      <c r="E436">
-        <v>3</v>
-      </c>
-      <c r="F436">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A437" t="s">
-        <v>17</v>
-      </c>
-      <c r="B437">
-        <v>184</v>
-      </c>
-      <c r="C437" t="s">
-        <v>5</v>
-      </c>
-      <c r="D437">
-        <v>3</v>
-      </c>
-      <c r="E437">
-        <v>1</v>
-      </c>
-      <c r="F437">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
-        <v>18</v>
-      </c>
-      <c r="B438">
-        <v>185</v>
-      </c>
-      <c r="C438" t="s">
-        <v>5</v>
-      </c>
-      <c r="D438">
-        <v>3</v>
-      </c>
-      <c r="E438">
-        <v>2</v>
-      </c>
-      <c r="F438">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A439" t="s">
-        <v>19</v>
-      </c>
-      <c r="B439">
-        <v>186</v>
-      </c>
-      <c r="C439" t="s">
-        <v>5</v>
-      </c>
-      <c r="D439">
-        <v>3</v>
-      </c>
-      <c r="E439">
-        <v>3</v>
-      </c>
-      <c r="F439">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A440" t="s">
-        <v>11</v>
-      </c>
-      <c r="B440">
-        <v>187</v>
-      </c>
-      <c r="C440" t="s">
-        <v>5</v>
-      </c>
-      <c r="D440">
-        <v>2</v>
-      </c>
-      <c r="E440">
-        <v>1</v>
-      </c>
-      <c r="F440">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
-        <v>12</v>
-      </c>
-      <c r="B441">
-        <v>188</v>
-      </c>
-      <c r="C441" t="s">
-        <v>5</v>
-      </c>
-      <c r="D441">
-        <v>2</v>
-      </c>
-      <c r="E441">
-        <v>2</v>
-      </c>
-      <c r="F441">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
-        <v>13</v>
-      </c>
-      <c r="B442">
-        <v>189</v>
-      </c>
-      <c r="C442" t="s">
-        <v>5</v>
-      </c>
-      <c r="D442">
-        <v>2</v>
-      </c>
-      <c r="E442">
-        <v>3</v>
-      </c>
-      <c r="F442">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
-        <v>14</v>
-      </c>
-      <c r="B443">
-        <v>190</v>
-      </c>
-      <c r="C443" t="s">
-        <v>5</v>
-      </c>
-      <c r="D443">
-        <v>4</v>
-      </c>
-      <c r="E443">
-        <v>1</v>
-      </c>
-      <c r="F443">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A444" t="s">
-        <v>15</v>
-      </c>
-      <c r="B444">
-        <v>191</v>
-      </c>
-      <c r="C444" t="s">
-        <v>5</v>
-      </c>
-      <c r="D444">
-        <v>4</v>
-      </c>
-      <c r="E444">
-        <v>2</v>
-      </c>
-      <c r="F444">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
-        <v>16</v>
-      </c>
-      <c r="B445">
-        <v>192</v>
-      </c>
-      <c r="C445" t="s">
-        <v>5</v>
-      </c>
-      <c r="D445">
-        <v>4</v>
-      </c>
-      <c r="E445">
-        <v>3</v>
-      </c>
-      <c r="F445">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A446" t="s">
-        <v>20</v>
-      </c>
-      <c r="B446">
-        <v>0</v>
-      </c>
-      <c r="C446" t="s">
-        <v>6</v>
-      </c>
-      <c r="D446">
-        <v>0</v>
-      </c>
-      <c r="E446">
-        <v>0</v>
-      </c>
-      <c r="F446">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A447" t="s">
-        <v>20</v>
-      </c>
-      <c r="B447">
-        <v>0</v>
-      </c>
-      <c r="C447" t="s">
-        <v>6</v>
-      </c>
-      <c r="D447">
-        <v>0</v>
-      </c>
-      <c r="E447">
-        <v>0</v>
-      </c>
-      <c r="F447">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A448" t="s">
-        <v>20</v>
-      </c>
-      <c r="B448">
-        <v>0</v>
-      </c>
-      <c r="C448" t="s">
-        <v>6</v>
-      </c>
-      <c r="D448">
-        <v>0</v>
-      </c>
-      <c r="E448">
-        <v>0</v>
-      </c>
-      <c r="F448">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
-        <v>20</v>
-      </c>
-      <c r="B449">
-        <v>0</v>
-      </c>
-      <c r="C449" t="s">
-        <v>6</v>
-      </c>
-      <c r="D449">
-        <v>0</v>
-      </c>
-      <c r="E449">
-        <v>0</v>
-      </c>
-      <c r="F449">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A450" t="s">
-        <v>20</v>
-      </c>
-      <c r="B450">
-        <v>0</v>
-      </c>
-      <c r="C450" t="s">
-        <v>6</v>
-      </c>
-      <c r="D450">
-        <v>0</v>
-      </c>
-      <c r="E450">
-        <v>0</v>
-      </c>
-      <c r="F450">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A451" t="s">
-        <v>20</v>
-      </c>
-      <c r="B451">
-        <v>0</v>
-      </c>
-      <c r="C451" t="s">
-        <v>6</v>
-      </c>
-      <c r="D451">
-        <v>0</v>
-      </c>
-      <c r="E451">
-        <v>0</v>
-      </c>
-      <c r="F451">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A452" t="s">
-        <v>20</v>
-      </c>
-      <c r="B452">
-        <v>0</v>
-      </c>
-      <c r="C452" t="s">
-        <v>6</v>
-      </c>
-      <c r="D452">
-        <v>0</v>
-      </c>
-      <c r="E452">
-        <v>0</v>
-      </c>
-      <c r="F452">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A453" t="s">
-        <v>20</v>
-      </c>
-      <c r="B453">
-        <v>0</v>
-      </c>
-      <c r="C453" t="s">
-        <v>6</v>
-      </c>
-      <c r="D453">
-        <v>0</v>
-      </c>
-      <c r="E453">
-        <v>0</v>
-      </c>
-      <c r="F453">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A454" t="s">
-        <v>20</v>
-      </c>
-      <c r="B454">
-        <v>0</v>
-      </c>
-      <c r="C454" t="s">
-        <v>6</v>
-      </c>
-      <c r="D454">
-        <v>0</v>
-      </c>
-      <c r="E454">
-        <v>0</v>
-      </c>
-      <c r="F454">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A455" t="s">
-        <v>20</v>
-      </c>
-      <c r="B455">
-        <v>0</v>
-      </c>
-      <c r="C455" t="s">
-        <v>6</v>
-      </c>
-      <c r="D455">
-        <v>0</v>
-      </c>
-      <c r="E455">
-        <v>0</v>
-      </c>
-      <c r="F455">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A456" t="s">
-        <v>20</v>
-      </c>
-      <c r="B456">
-        <v>0</v>
-      </c>
-      <c r="C456" t="s">
-        <v>6</v>
-      </c>
-      <c r="D456">
-        <v>0</v>
-      </c>
-      <c r="E456">
-        <v>0</v>
-      </c>
-      <c r="F456">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A457" t="s">
-        <v>20</v>
-      </c>
-      <c r="B457">
-        <v>0</v>
-      </c>
-      <c r="C457" t="s">
-        <v>6</v>
-      </c>
-      <c r="D457">
-        <v>0</v>
-      </c>
-      <c r="E457">
-        <v>0</v>
-      </c>
-      <c r="F457">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A458" t="s">
-        <v>24</v>
-      </c>
-      <c r="B458">
-        <v>169</v>
-      </c>
-      <c r="C458" t="s">
-        <v>7</v>
-      </c>
-      <c r="D458">
-        <v>0</v>
-      </c>
-      <c r="E458">
-        <v>1</v>
-      </c>
-      <c r="F458">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A459" t="s">
-        <v>31</v>
-      </c>
-      <c r="B459">
-        <v>170</v>
-      </c>
-      <c r="C459" t="s">
-        <v>7</v>
-      </c>
-      <c r="D459">
-        <v>0</v>
-      </c>
-      <c r="E459">
-        <v>2</v>
-      </c>
-      <c r="F459">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A460" t="s">
-        <v>32</v>
-      </c>
-      <c r="B460">
-        <v>171</v>
-      </c>
-      <c r="C460" t="s">
-        <v>7</v>
-      </c>
-      <c r="D460">
-        <v>0</v>
-      </c>
-      <c r="E460">
-        <v>3</v>
-      </c>
-      <c r="F460">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A461" t="s">
-        <v>23</v>
-      </c>
-      <c r="B461">
-        <v>172</v>
-      </c>
-      <c r="C461" t="s">
-        <v>7</v>
-      </c>
-      <c r="D461">
-        <v>0</v>
-      </c>
-      <c r="E461">
-        <v>1</v>
-      </c>
-      <c r="F461">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A462" t="s">
-        <v>24</v>
-      </c>
-      <c r="B462">
-        <v>173</v>
-      </c>
-      <c r="C462" t="s">
-        <v>7</v>
-      </c>
-      <c r="D462">
-        <v>0</v>
-      </c>
-      <c r="E462">
-        <v>2</v>
-      </c>
-      <c r="F462">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A463" t="s">
-        <v>29</v>
-      </c>
-      <c r="B463">
-        <v>174</v>
-      </c>
-      <c r="C463" t="s">
-        <v>7</v>
-      </c>
-      <c r="D463">
-        <v>0</v>
-      </c>
-      <c r="E463">
-        <v>3</v>
-      </c>
-      <c r="F463">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A464" t="s">
-        <v>28</v>
-      </c>
-      <c r="B464">
-        <v>175</v>
-      </c>
-      <c r="C464" t="s">
-        <v>7</v>
-      </c>
-      <c r="D464">
-        <v>0</v>
-      </c>
-      <c r="E464">
-        <v>1</v>
-      </c>
-      <c r="F464">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A465" t="s">
-        <v>22</v>
-      </c>
-      <c r="B465">
-        <v>176</v>
-      </c>
-      <c r="C465" t="s">
-        <v>7</v>
-      </c>
-      <c r="D465">
-        <v>0</v>
-      </c>
-      <c r="E465">
-        <v>2</v>
-      </c>
-      <c r="F465">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A466" t="s">
-        <v>27</v>
-      </c>
-      <c r="B466">
-        <v>177</v>
-      </c>
-      <c r="C466" t="s">
-        <v>7</v>
-      </c>
-      <c r="D466">
-        <v>0</v>
-      </c>
-      <c r="E466">
-        <v>3</v>
-      </c>
-      <c r="F466">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A467" t="s">
-        <v>32</v>
-      </c>
-      <c r="B467">
-        <v>178</v>
-      </c>
-      <c r="C467" t="s">
-        <v>7</v>
-      </c>
-      <c r="D467">
-        <v>0</v>
-      </c>
-      <c r="E467">
-        <v>1</v>
-      </c>
-      <c r="F467">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A468" t="s">
-        <v>31</v>
-      </c>
-      <c r="B468">
-        <v>179</v>
-      </c>
-      <c r="C468" t="s">
-        <v>7</v>
-      </c>
-      <c r="D468">
-        <v>0</v>
-      </c>
-      <c r="E468">
-        <v>2</v>
-      </c>
-      <c r="F468">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A469" t="s">
-        <v>27</v>
-      </c>
-      <c r="B469">
-        <v>180</v>
-      </c>
-      <c r="C469" t="s">
-        <v>7</v>
-      </c>
-      <c r="D469">
-        <v>0</v>
-      </c>
-      <c r="E469">
-        <v>3</v>
-      </c>
-      <c r="F469">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A470" t="s">
-        <v>21</v>
-      </c>
-      <c r="B470">
-        <v>181</v>
-      </c>
-      <c r="C470" t="s">
-        <v>7</v>
-      </c>
-      <c r="D470">
-        <v>0</v>
-      </c>
-      <c r="E470">
-        <v>1</v>
-      </c>
-      <c r="F470">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>30</v>
-      </c>
-      <c r="B471">
-        <v>182</v>
-      </c>
-      <c r="C471" t="s">
-        <v>7</v>
-      </c>
-      <c r="D471">
-        <v>0</v>
-      </c>
-      <c r="E471">
-        <v>2</v>
-      </c>
-      <c r="F471">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A472" t="s">
-        <v>25</v>
-      </c>
-      <c r="B472">
-        <v>183</v>
-      </c>
-      <c r="C472" t="s">
-        <v>7</v>
-      </c>
-      <c r="D472">
-        <v>0</v>
-      </c>
-      <c r="E472">
-        <v>3</v>
-      </c>
-      <c r="F472">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A473" t="s">
-        <v>25</v>
-      </c>
-      <c r="B473">
-        <v>184</v>
-      </c>
-      <c r="C473" t="s">
-        <v>7</v>
-      </c>
-      <c r="D473">
-        <v>0</v>
-      </c>
-      <c r="E473">
-        <v>1</v>
-      </c>
-      <c r="F473">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A474" t="s">
-        <v>28</v>
-      </c>
-      <c r="B474">
-        <v>185</v>
-      </c>
-      <c r="C474" t="s">
-        <v>7</v>
-      </c>
-      <c r="D474">
-        <v>0</v>
-      </c>
-      <c r="E474">
-        <v>2</v>
-      </c>
-      <c r="F474">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A475" t="s">
-        <v>27</v>
-      </c>
-      <c r="B475">
-        <v>186</v>
-      </c>
-      <c r="C475" t="s">
-        <v>7</v>
-      </c>
-      <c r="D475">
-        <v>0</v>
-      </c>
-      <c r="E475">
-        <v>3</v>
-      </c>
-      <c r="F475">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A476" t="s">
-        <v>26</v>
-      </c>
-      <c r="B476">
-        <v>187</v>
-      </c>
-      <c r="C476" t="s">
-        <v>7</v>
-      </c>
-      <c r="D476">
-        <v>0</v>
-      </c>
-      <c r="E476">
-        <v>1</v>
-      </c>
-      <c r="F476">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A477" t="s">
-        <v>26</v>
-      </c>
-      <c r="B477">
-        <v>188</v>
-      </c>
-      <c r="C477" t="s">
-        <v>7</v>
-      </c>
-      <c r="D477">
-        <v>0</v>
-      </c>
-      <c r="E477">
-        <v>2</v>
-      </c>
-      <c r="F477">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A478" t="s">
-        <v>21</v>
-      </c>
-      <c r="B478">
-        <v>189</v>
-      </c>
-      <c r="C478" t="s">
-        <v>7</v>
-      </c>
-      <c r="D478">
-        <v>0</v>
-      </c>
-      <c r="E478">
-        <v>3</v>
-      </c>
-      <c r="F478">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A479" t="s">
-        <v>30</v>
-      </c>
-      <c r="B479">
-        <v>190</v>
-      </c>
-      <c r="C479" t="s">
-        <v>7</v>
-      </c>
-      <c r="D479">
-        <v>0</v>
-      </c>
-      <c r="E479">
-        <v>1</v>
-      </c>
-      <c r="F479">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A480" t="s">
-        <v>30</v>
-      </c>
-      <c r="B480">
-        <v>191</v>
-      </c>
-      <c r="C480" t="s">
-        <v>7</v>
-      </c>
-      <c r="D480">
-        <v>0</v>
-      </c>
-      <c r="E480">
-        <v>2</v>
-      </c>
-      <c r="F480">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A481" t="s">
-        <v>24</v>
-      </c>
-      <c r="B481">
-        <v>192</v>
-      </c>
-      <c r="C481" t="s">
-        <v>7</v>
-      </c>
-      <c r="D481">
-        <v>0</v>
-      </c>
-      <c r="E481">
-        <v>3</v>
-      </c>
-      <c r="F481">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>